<commit_message>
Se agragaron las entradas de datos del excel
</commit_message>
<xml_diff>
--- a/MetproproyectoFinal.xlsx
+++ b/MetproproyectoFinal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Samael Flores\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Samael Flores\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94634FA5-1337-4676-B50C-467479942A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B5A6C3-7CE6-493B-B877-D94E87D904FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1110" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1110" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t>Identificador</t>
   </si>
@@ -102,6 +102,48 @@
   </si>
   <si>
     <t>Formato</t>
+  </si>
+  <si>
+    <t>Nombre completo</t>
+  </si>
+  <si>
+    <t>Tipo de Moneda</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>Nomina</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Centro de costo</t>
+  </si>
+  <si>
+    <t>Fecha de nacimineto</t>
+  </si>
+  <si>
+    <t>Fecha de registo</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Numero de seguro</t>
+  </si>
+  <si>
+    <t>Interes</t>
+  </si>
+  <si>
+    <t>Cedula</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Global</t>
   </si>
 </sst>
 </file>
@@ -150,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -285,11 +327,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -330,6 +432,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,8 +728,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:J1048574"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -657,7 +771,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="2:10" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -686,143 +800,247 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+    <row r="5" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+    <row r="6" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+    <row r="7" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
+    <row r="8" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+    <row r="9" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+    <row r="10" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+    <row r="11" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+    <row r="12" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+    <row r="13" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+    <row r="14" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+    <row r="15" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+    <row r="16" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+    <row r="17" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -833,7 +1051,7 @@
       <c r="B18" s="5"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -912,10 +1130,10 @@
     <mergeCell ref="B2:J2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C21" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$B$1048570:$B$1048572</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D21" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D21" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$A$1048570:$A$1048574</formula1>
     </dataValidation>
   </dataValidations>
@@ -929,7 +1147,7 @@
   <dimension ref="B1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="A1:E20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="A3:F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se efectuan algunos cambios en el excel
</commit_message>
<xml_diff>
--- a/MetproproyectoFinal.xlsx
+++ b/MetproproyectoFinal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c4bcae6ddc20b51/Desktop/SERFIGSA/Cronograma-de-pago-SERFIGSA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maurita\Desktop\Cronograma-de-pago-SERFIGSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{70B5A6C3-7CE6-493B-B877-D94E87D904FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D80A6478-8E2F-4818-BFC7-13BD86484AD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A9CE0E-ECE0-4E3E-B498-7B3942170414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +268,20 @@
       <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -483,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -537,7 +551,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,15 +576,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1457324</xdr:colOff>
+      <xdr:colOff>1495424</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
+      <xdr:colOff>561974</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -583,7 +599,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4190999" y="1733550"/>
+          <a:off x="4229099" y="1752600"/>
           <a:ext cx="600075" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -592,7 +608,7 @@
         <a:noFill/>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="tx1"/>
+            <a:srgbClr val="FF0000"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
@@ -617,7 +633,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -893,7 +913,7 @@
   <dimension ref="A2:J1048574"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1010,7 +1030,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>38</v>
@@ -1029,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>38</v>
@@ -1048,7 +1068,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>38</v>
@@ -1200,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>38</v>
@@ -1310,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,35 +1377,35 @@
       <c r="B5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
@@ -1459,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se corrigen cambios en el excel
</commit_message>
<xml_diff>
--- a/MetproproyectoFinal.xlsx
+++ b/MetproproyectoFinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maurita\Desktop\Cronograma-de-pago-SERFIGSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A9CE0E-ECE0-4E3E-B498-7B3942170414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB40BDA8-D550-4667-8F9B-0389E64549AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Identificador</t>
   </si>
@@ -104,45 +104,6 @@
     <t>Formato</t>
   </si>
   <si>
-    <t>Nombre completo</t>
-  </si>
-  <si>
-    <t>Tipo de Moneda</t>
-  </si>
-  <si>
-    <t>Monto</t>
-  </si>
-  <si>
-    <t>Nomina</t>
-  </si>
-  <si>
-    <t>Departamento</t>
-  </si>
-  <si>
-    <t>Centro de costo</t>
-  </si>
-  <si>
-    <t>Fecha de nacimineto</t>
-  </si>
-  <si>
-    <t>Fecha de registo</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Numero de seguro</t>
-  </si>
-  <si>
-    <t>Interes</t>
-  </si>
-  <si>
-    <t>Cedula</t>
-  </si>
-  <si>
-    <t>Telefono</t>
-  </si>
-  <si>
     <t>Global</t>
   </si>
   <si>
@@ -231,6 +192,42 @@
   </si>
   <si>
     <t>Interes Aplicado:%10</t>
+  </si>
+  <si>
+    <t>nombreCompleto</t>
+  </si>
+  <si>
+    <t>monto</t>
+  </si>
+  <si>
+    <t>interes</t>
+  </si>
+  <si>
+    <t>cedula</t>
+  </si>
+  <si>
+    <t>nomina</t>
+  </si>
+  <si>
+    <t>numeroDeSeguro</t>
+  </si>
+  <si>
+    <t>departamento</t>
+  </si>
+  <si>
+    <t>centroDeCosto</t>
+  </si>
+  <si>
+    <t>fechaNac</t>
+  </si>
+  <si>
+    <t>fechaReg</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>telefono</t>
   </si>
 </sst>
 </file>
@@ -524,6 +521,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,9 +551,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +910,7 @@
   <dimension ref="A2:J1048574"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -932,17 +929,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
@@ -986,7 +983,7 @@
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>5</v>
@@ -995,7 +992,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
@@ -1005,7 +1002,7 @@
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>5</v>
@@ -1014,7 +1011,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
@@ -1024,7 +1021,7 @@
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>5</v>
@@ -1033,7 +1030,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
@@ -1043,7 +1040,7 @@
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>5</v>
@@ -1052,7 +1049,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1062,7 +1059,7 @@
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>5</v>
@@ -1071,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -1081,7 +1078,7 @@
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>5</v>
@@ -1090,7 +1087,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -1100,7 +1097,7 @@
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>5</v>
@@ -1109,7 +1106,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1119,7 +1116,7 @@
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>5</v>
@@ -1128,7 +1125,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1138,7 +1135,7 @@
     </row>
     <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>5</v>
@@ -1147,7 +1144,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1157,7 +1154,7 @@
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>5</v>
@@ -1166,7 +1163,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1176,7 +1173,7 @@
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>5</v>
@@ -1185,7 +1182,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1195,7 +1192,7 @@
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>5</v>
@@ -1204,7 +1201,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1214,7 +1211,7 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>5</v>
@@ -1223,7 +1220,7 @@
         <v>12</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1330,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
@@ -1342,11 +1339,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="2:4" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
@@ -1366,53 +1363,53 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="22"/>
+        <v>27</v>
+      </c>
+      <c r="C5" s="13"/>
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="21"/>
+        <v>28</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="21"/>
+        <v>30</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -1479,7 +1476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1492,12 +1489,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1510,119 +1507,119 @@
         <v>23</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="20"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>